<commit_message>
changes made second commit
</commit_message>
<xml_diff>
--- a/Excel/PluginLive Automation.xlsx
+++ b/Excel/PluginLive Automation.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PluginLive Automation\PluginLive Automation\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ICANIO-10090\Desktop\Project\PluginLive-Automation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D546385-FB1F-4D55-B4E8-B0A668C98E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0F6C23-B0DB-4CDA-A65C-0781F1436684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{2E2C8FCF-06E3-4FE5-BF9E-BD4ED11DFCB5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="4" xr2:uid="{2E2C8FCF-06E3-4FE5-BF9E-BD4ED11DFCB5}"/>
   </bookViews>
   <sheets>
     <sheet name="CorporateLogin" sheetId="1" r:id="rId1"/>
     <sheet name="JobDetails" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
-    <sheet name="EligibilityCriteria" sheetId="4" r:id="rId4"/>
+    <sheet name="CTCandJobLocation" sheetId="3" r:id="rId3"/>
+    <sheet name="Questionnaire" sheetId="5" r:id="rId4"/>
+    <sheet name="InterviewWorkflow" sheetId="6" r:id="rId5"/>
+    <sheet name="EligibilityCriteria" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>priya.t+1@icanio.com</t>
   </si>
@@ -87,9 +89,6 @@
     <t>workfromOfz</t>
   </si>
   <si>
-    <t>Bachelor Of Computer Applications</t>
-  </si>
-  <si>
     <t>B.E - Computer Science Engineering</t>
   </si>
   <si>
@@ -136,6 +135,84 @@
   </si>
   <si>
     <t>Javascript Frameworks</t>
+  </si>
+  <si>
+    <t>year1</t>
+  </si>
+  <si>
+    <t>year2</t>
+  </si>
+  <si>
+    <t>year3</t>
+  </si>
+  <si>
+    <t>year4</t>
+  </si>
+  <si>
+    <t>year5</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>option1</t>
+  </si>
+  <si>
+    <t>option2</t>
+  </si>
+  <si>
+    <t>Are you Okay to Relocate to Chennai?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Roundname1</t>
+  </si>
+  <si>
+    <t>Assessment</t>
+  </si>
+  <si>
+    <t>Round1Description</t>
+  </si>
+  <si>
+    <t>All The Best Do Well</t>
+  </si>
+  <si>
+    <t>Roundname2</t>
+  </si>
+  <si>
+    <t>Technical Round</t>
+  </si>
+  <si>
+    <t>Must Have knowledge regarding the job position</t>
+  </si>
+  <si>
+    <t>Round2Description</t>
+  </si>
+  <si>
+    <t>HR Discussion</t>
+  </si>
+  <si>
+    <t>Discussion regarding the Location, Shift and Package also About the Company</t>
+  </si>
+  <si>
+    <t>Roundname3</t>
+  </si>
+  <si>
+    <t>Round3Description</t>
+  </si>
+  <si>
+    <t>Bachelor Of Engineeringg</t>
+  </si>
+  <si>
+    <t>clgName</t>
+  </si>
+  <si>
+    <t>Demo College of engineering</t>
   </si>
 </sst>
 </file>
@@ -530,7 +607,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -565,9 +642,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -621,10 +698,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -634,7 +711,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>18</v>
@@ -648,10 +725,10 @@
         <v>400000</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -660,16 +737,116 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A97F707-8020-4BB4-AC05-06DB46171DA7}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F5757F-6DC3-4FF3-974D-826714A175FA}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C39547-08B4-41EA-B687-F488873DD587}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A97F707-8020-4BB4-AC05-06DB46171DA7}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -677,48 +854,78 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>35</v>
+      <c r="I2">
+        <v>2020</v>
+      </c>
+      <c r="J2">
+        <v>2021</v>
+      </c>
+      <c r="K2">
+        <v>2022</v>
+      </c>
+      <c r="L2">
+        <v>2023</v>
+      </c>
+      <c r="M2">
+        <v>2024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>